<commit_message>
fixed bugs in sim
</commit_message>
<xml_diff>
--- a/Results/RiskTransfer/RiskTransfer_stch.tab.xlsx
+++ b/Results/RiskTransfer/RiskTransfer_stch.tab.xlsx
@@ -215,19 +215,19 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>274.56954909549495</v>
+        <v>267.48369273734477</v>
       </c>
       <c r="D3" t="n">
-        <v>213.7127809409429</v>
+        <v>206.6269245827927</v>
       </c>
       <c r="E3" t="n">
-        <v>133.585431955404</v>
+        <v>126.4995755972538</v>
       </c>
       <c r="F3" t="n">
-        <v>7.13001888289903</v>
+        <v>0.04416252474882043</v>
       </c>
       <c r="G3" t="n">
-        <v>80.5341134675206</v>
+        <v>73.4482571093704</v>
       </c>
       <c r="H3" t="n">
         <v>212.28707157749554</v>
@@ -236,16 +236,16 @@
         <v>206.58276205804387</v>
       </c>
       <c r="J3" t="n">
-        <v>140.98411714009094</v>
+        <v>140.98411714009097</v>
       </c>
       <c r="K3" t="n">
         <v>80.1273489855389</v>
       </c>
       <c r="L3" t="n">
-        <v>1.0553854194756576</v>
+        <v>1.114502688838678</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5998210120119125</v>
+        <v>0.6334199036417827</v>
       </c>
     </row>
   </sheetData>
@@ -349,37 +349,37 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>30.129397037560732</v>
+        <v>23.04354067941053</v>
       </c>
       <c r="D3" t="n">
-        <v>26.138651761496064</v>
+        <v>19.05279540334587</v>
       </c>
       <c r="E3" t="n">
-        <v>20.44927769861444</v>
+        <v>13.363421340464242</v>
       </c>
       <c r="F3" t="n">
-        <v>13.380794166562161</v>
+        <v>6.2949378084119605</v>
       </c>
       <c r="G3" t="n">
-        <v>18.5032005689215</v>
+        <v>11.417344210771299</v>
       </c>
       <c r="H3" t="n">
         <v>10.906923519843739</v>
       </c>
       <c r="I3" t="n">
-        <v>12.757857594933903</v>
+        <v>12.757857594933908</v>
       </c>
       <c r="J3" t="n">
-        <v>9.680119338946291</v>
+        <v>9.680119338946287</v>
       </c>
       <c r="K3" t="n">
-        <v>5.6893740628816225</v>
+        <v>5.689374062881626</v>
       </c>
       <c r="L3" t="n">
-        <v>0.47337218857378893</v>
+        <v>0.7243743269274185</v>
       </c>
       <c r="M3" t="n">
-        <v>0.278218827419372</v>
+        <v>0.42574232435927817</v>
       </c>
     </row>
   </sheetData>
@@ -483,19 +483,19 @@
         <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>165.4997434355252</v>
+        <v>154.0160415479052</v>
       </c>
       <c r="D3" t="n">
-        <v>133.71596447484893</v>
+        <v>122.23226258722894</v>
       </c>
       <c r="E3" t="n">
-        <v>92.31092720787296</v>
+        <v>80.82722532025296</v>
       </c>
       <c r="F3" t="n">
-        <v>23.99979048783044</v>
+        <v>12.516088600210448</v>
       </c>
       <c r="G3" t="n">
-        <v>64.12024981509732</v>
+        <v>52.63654792747733</v>
       </c>
       <c r="H3" t="n">
         <v>111.06988048708574</v>
@@ -504,16 +504,16 @@
         <v>109.7161739870185</v>
       </c>
       <c r="J3" t="n">
-        <v>73.18881622765224</v>
+        <v>73.18881622765223</v>
       </c>
       <c r="K3" t="n">
-        <v>41.40503726697597</v>
+        <v>41.40503726697598</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7928510571975942</v>
+        <v>0.9054970764821395</v>
       </c>
       <c r="M3" t="n">
-        <v>0.44853885145944705</v>
+        <v>0.5122659735370265</v>
       </c>
     </row>
   </sheetData>
@@ -617,19 +617,19 @@
         <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>280.9651964540591</v>
+        <v>273.87934009590884</v>
       </c>
       <c r="D3" t="n">
-        <v>218.11611381214428</v>
+        <v>211.0302574539941</v>
       </c>
       <c r="E3" t="n">
-        <v>135.09906862500065</v>
+        <v>128.01321226685042</v>
       </c>
       <c r="F3" t="n">
-        <v>8.503913902106781</v>
+        <v>1.4180575439565928</v>
       </c>
       <c r="G3" t="n">
-        <v>83.58828382447483</v>
+        <v>76.50242746632463</v>
       </c>
       <c r="H3" t="n">
         <v>214.14349787211336</v>
@@ -641,13 +641,13 @@
         <v>145.86612782905843</v>
       </c>
       <c r="K3" t="n">
-        <v>83.01704518714362</v>
+        <v>83.01704518714368</v>
       </c>
       <c r="L3" t="n">
-        <v>1.07969750875148</v>
+        <v>1.1394615074965282</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6144901369940383</v>
+        <v>0.6485037264285674</v>
       </c>
     </row>
   </sheetData>
@@ -751,37 +751,37 @@
         <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>34.78462317102317</v>
+        <v>27.698766812872968</v>
       </c>
       <c r="D3" t="n">
-        <v>29.722400794018398</v>
+        <v>22.6365444358682</v>
       </c>
       <c r="E3" t="n">
-        <v>23.12082927088745</v>
+        <v>16.034972912737253</v>
       </c>
       <c r="F3" t="n">
-        <v>14.98968394611616</v>
+        <v>7.90382758796596</v>
       </c>
       <c r="G3" t="n">
-        <v>21.208047319986935</v>
+        <v>14.122190961836736</v>
       </c>
       <c r="H3" t="n">
-        <v>12.051279318205646</v>
+        <v>12.05127931820565</v>
       </c>
       <c r="I3" t="n">
-        <v>14.732716847902237</v>
+        <v>14.732716847902239</v>
       </c>
       <c r="J3" t="n">
-        <v>11.663793900135719</v>
+        <v>11.663793900135715</v>
       </c>
       <c r="K3" t="n">
         <v>6.601571523130946</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5044712611074968</v>
+        <v>0.7273971689014</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2855248592421078</v>
+        <v>0.4116983270914689</v>
       </c>
     </row>
   </sheetData>
@@ -885,37 +885,37 @@
         <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>172.6554928640267</v>
+        <v>161.17179097640673</v>
       </c>
       <c r="D3" t="n">
-        <v>138.54763120224948</v>
+        <v>127.0639293146295</v>
       </c>
       <c r="E3" t="n">
-        <v>93.64965379214469</v>
+        <v>82.16595190452469</v>
       </c>
       <c r="F3" t="n">
-        <v>24.609971855739985</v>
+        <v>13.126269968120003</v>
       </c>
       <c r="G3" t="n">
-        <v>67.18090834208438</v>
+        <v>55.697206454464386</v>
       </c>
       <c r="H3" t="n">
         <v>112.91796305278825</v>
       </c>
       <c r="I3" t="n">
-        <v>113.93765934650949</v>
+        <v>113.9376593465095</v>
       </c>
       <c r="J3" t="n">
-        <v>79.00583907188202</v>
+        <v>79.00583907188204</v>
       </c>
       <c r="K3" t="n">
-        <v>44.89797741010479</v>
+        <v>44.897977410104815</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8436319396037</v>
+        <v>0.9615398743713863</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4794249160787696</v>
+        <v>0.5464304419216786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>